<commit_message>
el bot de discord responde a los mensajes
</commit_message>
<xml_diff>
--- a/nike.xlsx
+++ b/nike.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF97858F-4A7C-4552-BED2-323226E1A211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Resultados" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Resultados" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>Nombre</t>
   </si>
@@ -26,59 +22,119 @@
     <t>Fecha</t>
   </si>
   <si>
+    <t>Foto</t>
+  </si>
+  <si>
     <t>W Dunk High Lx</t>
   </si>
   <si>
+    <t>$136.990</t>
+  </si>
+  <si>
     <t>Disponible el 25-01 a las 11:00</t>
   </si>
   <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/630131-1000-1000/DQ7575_300_A_PREM.jpg?v=638047234916100000</t>
+  </si>
+  <si>
     <t>Air Jordan 1 Retro Low</t>
   </si>
   <si>
+    <t>$159.990</t>
+  </si>
+  <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/623368-1000-1000/DZ7292_200_A_PREM.jpg?v=638035163436270000</t>
+  </si>
+  <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/620337-1000-1000/DZ7327_001_A_PREM.jpg?v=638029250777100000</t>
+  </si>
+  <si>
     <t>W Air Force 1 Lx</t>
   </si>
   <si>
+    <t>$134.990</t>
+  </si>
+  <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/620296-1000-1000/DQ7580_700_A_PREM.jpg?v=638029250206630000</t>
+  </si>
+  <si>
     <t>Terminator High</t>
   </si>
   <si>
+    <t>$149.990</t>
+  </si>
+  <si>
     <t>Disponible el 26-01 a las 11:00</t>
   </si>
   <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/648965-1000-1000/FD0650_100_A_PREM.jpg?v=638091338990600000</t>
+  </si>
+  <si>
     <t>W Dunk Low Lx</t>
   </si>
   <si>
+    <t>$129.990</t>
+  </si>
+  <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/648818-1000-1000/DV3054_600_A_PREM.jpg?v=638091337049600000</t>
+  </si>
+  <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/648805-1000-1000/DV3054_001_A_PREM.jpg?v=638091336897030000</t>
+  </si>
+  <si>
     <t>Air max 1 Prm</t>
   </si>
   <si>
+    <t>$164.990</t>
+  </si>
+  <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/635930-1000-1000/DZ0482_200_A_PREM.jpg?v=638068187691070000</t>
+  </si>
+  <si>
     <t>Air max 1</t>
   </si>
   <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/635924-1000-1000/DZ0482_001_A_PREM.jpg?v=638068174946030000</t>
+  </si>
+  <si>
     <t>Disponible el 27-01 a las 11:00</t>
   </si>
   <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/638482-1000-1000/DR0148_101_A_PREM-hei-3144-wid-3144-fmt.jpg?v=638078771596430000</t>
+  </si>
+  <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/638457-1000-1000/DR0148_100_A_PREM-hei-3144-wid-3144-fmt.jpg?v=638078771436000000</t>
+  </si>
+  <si>
     <t>W Air Force 1 Lxx</t>
   </si>
   <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/625045-1000-1000/DX1193_200_A_PREM.jpg?v=638036904577830000</t>
+  </si>
+  <si>
     <t>Lebron XX</t>
   </si>
   <si>
+    <t>$199.990</t>
+  </si>
+  <si>
     <t>Disponible el 30-01 a las 11:00</t>
+  </si>
+  <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/620585-1000-1000/DJ5423_100_A_PREM.jpg?v=638029254372400000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,9 +157,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,21 +497,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-  </cols>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,152 +511,194 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>136.99</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
-        <v>159.99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>136.99</v>
-      </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
-        <v>134.99</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>149.99</v>
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
-        <v>129.99</v>
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>129.99</v>
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>164.99</v>
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
-        <v>164.99</v>
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1">
-        <v>149.99</v>
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
       </c>
       <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1">
-        <v>149.99</v>
+      <c r="B12" t="s">
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
-        <v>134.99</v>
-      </c>
       <c r="C13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1">
-        <v>199.99</v>
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Avance con la ejecucion del bot completo
</commit_message>
<xml_diff>
--- a/nike.xlsx
+++ b/nike.xlsx
@@ -25,16 +25,28 @@
     <t>Foto</t>
   </si>
   <si>
+    <t>W Air Force 1 Lx</t>
+  </si>
+  <si>
+    <t>$134.990</t>
+  </si>
+  <si>
+    <t>Ya esta disponible</t>
+  </si>
+  <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/620296-1000-1000/DQ7580_700_A_PREM.jpg?v=638029250206630000</t>
+  </si>
+  <si>
     <t>W Dunk High Lx</t>
   </si>
   <si>
     <t>$136.990</t>
   </si>
   <si>
-    <t>Disponible el 25-01 a las 11:00</t>
-  </si>
-  <si>
-    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/630131-1000-1000/DQ7575_300_A_PREM.jpg?v=638047234916100000</t>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/620337-1000-1000/DZ7327_001_A_PREM.jpg?v=638029250777100000</t>
+  </si>
+  <si>
+    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/630132-1000-1000/DQ7575_300_A_PREM.jpg?v=638047234928730000</t>
   </si>
   <si>
     <t>Air Jordan 1 Retro Low</t>
@@ -44,18 +56,6 @@
   </si>
   <si>
     <t>https://nikeclprod.vteximg.com.br/arquivos/ids/623368-1000-1000/DZ7292_200_A_PREM.jpg?v=638035163436270000</t>
-  </si>
-  <si>
-    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/620337-1000-1000/DZ7327_001_A_PREM.jpg?v=638029250777100000</t>
-  </si>
-  <si>
-    <t>W Air Force 1 Lx</t>
-  </si>
-  <si>
-    <t>$134.990</t>
-  </si>
-  <si>
-    <t>https://nikeclprod.vteximg.com.br/arquivos/ids/620296-1000-1000/DQ7580_700_A_PREM.jpg?v=638029250206630000</t>
   </si>
   <si>
     <t>Terminator High</t>
@@ -545,10 +545,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -674,7 +674,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>

</xml_diff>